<commit_message>
Cambios de sisia ok
</commit_message>
<xml_diff>
--- a/Documentacion/Usuariosv4.xlsx
+++ b/Documentacion/Usuariosv4.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5772" uniqueCount="1393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5780" uniqueCount="1393">
   <si>
     <t>id_usuario</t>
   </si>
@@ -33506,7 +33506,7 @@
   <dimension ref="A1:M156"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A2"/>
+      <selection sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -33516,8 +33516,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="34" t="s">
-        <v>403</v>
+      <c r="A1" s="5" t="s">
+        <v>154</v>
       </c>
       <c r="B1" s="49" t="s">
         <v>502</v>
@@ -33558,7 +33558,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>405</v>
+        <v>146</v>
       </c>
       <c r="B2" s="49" t="s">
         <v>502</v>
@@ -33598,14 +33598,86 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="5"/>
-      <c r="B3" s="49"/>
-      <c r="F3" s="59"/>
+      <c r="A3" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="B3" s="49" t="s">
+        <v>502</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>103</v>
+      </c>
+      <c r="F3" s="59" t="s">
+        <v>1390</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>152</v>
+      </c>
+      <c r="I3" t="s">
+        <v>1392</v>
+      </c>
+      <c r="J3">
+        <v>10</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>9</v>
+      </c>
+      <c r="M3">
+        <v>7</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="5"/>
-      <c r="B4" s="49"/>
-      <c r="F4" s="59"/>
+      <c r="A4" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B4" s="49" t="s">
+        <v>502</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>105</v>
+      </c>
+      <c r="F4" s="59" t="s">
+        <v>1390</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <v>152</v>
+      </c>
+      <c r="I4" t="s">
+        <v>1392</v>
+      </c>
+      <c r="J4">
+        <v>10</v>
+      </c>
+      <c r="K4">
+        <v>2</v>
+      </c>
+      <c r="L4">
+        <v>9</v>
+      </c>
+      <c r="M4">
+        <v>8</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>

</xml_diff>